<commit_message>
DB UML update final
Finaler DB Entwurf
</commit_message>
<xml_diff>
--- a/Mockups und Struktur/Datenbanken UML.xlsx
+++ b/Mockups und Struktur/Datenbanken UML.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Honnullul\Dropbox\Studium\PRG\MyMedia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Honnullul\Dropbox\Studium\PRG\mymedia\Mockups und Struktur\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="24">
   <si>
     <t>Account</t>
   </si>
@@ -68,18 +68,12 @@
     <t>Kontakte</t>
   </si>
   <si>
-    <t>Medien und Kontakte mit Kommata getrennt</t>
-  </si>
-  <si>
     <t>&gt; Account.ID</t>
   </si>
   <si>
     <t>Ausleiher</t>
   </si>
   <si>
-    <t>1. Medium erstellen, dann zu Account hinzufügen</t>
-  </si>
-  <si>
     <t>Beschreibung</t>
   </si>
   <si>
@@ -95,10 +89,13 @@
     <t>Preview</t>
   </si>
   <si>
-    <t>&gt; Nutzermedien.ID</t>
-  </si>
-  <si>
     <t>Kursive Felder können leer sein</t>
+  </si>
+  <si>
+    <t>User1</t>
+  </si>
+  <si>
+    <t>User2</t>
   </si>
 </sst>
 </file>
@@ -234,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -246,12 +243,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
@@ -259,6 +250,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -539,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,31 +554,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="D1" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="12"/>
-      <c r="G1" s="11" t="s">
+      <c r="A1" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="D1" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="19"/>
+      <c r="G1" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="12"/>
-      <c r="J1" s="11" t="s">
+      <c r="H1" s="19"/>
+      <c r="J1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="12"/>
+      <c r="K1" s="19"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
@@ -602,11 +602,14 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>5</v>
+      <c r="A3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>2</v>
@@ -615,7 +618,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>4</v>
@@ -629,17 +632,11 @@
       <c r="J3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="14" t="s">
+      <c r="K3" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>9</v>
-      </c>
       <c r="D4" s="4" t="s">
         <v>2</v>
       </c>
@@ -647,7 +644,7 @@
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>4</v>
@@ -657,77 +654,83 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="20"/>
+      <c r="B5" s="20"/>
+      <c r="D5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="15" t="s">
+      <c r="H5" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="13" t="s">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="G6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="H6" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G7" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" s="17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G7" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="H7" s="19" t="s">
-        <v>22</v>
-      </c>
-    </row>
+      <c r="H7" s="17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="19"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>14</v>
+      <c r="G12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>17</v>
+      <c r="G13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G14" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:B1"/>
+  <mergeCells count="5">
+    <mergeCell ref="G11:H11"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="D1:E1"/>
+    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>